<commit_message>
Adding new data to designer
</commit_message>
<xml_diff>
--- a/allData.xlsx
+++ b/allData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzakr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZakrzewskiJakub\source\repos\Zakrzewiaczek\Weather-Rider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7988CF1-A67F-4837-ABE9-EE411C9D99F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F92743-AAC5-4201-9347-3E18BEA56EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{501DA96D-EA6F-4FF1-BC3F-B1390DEB246D}"/>
   </bookViews>
@@ -101,9 +101,6 @@
     <t>apparent_temperature</t>
   </si>
   <si>
-    <t>precipation</t>
-  </si>
-  <si>
     <t>rain</t>
   </si>
   <si>
@@ -567,6 +564,9 @@
   </si>
   <si>
     <t>ragweed_pollen</t>
+  </si>
+  <si>
+    <t>precipitation</t>
   </si>
 </sst>
 </file>
@@ -726,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -734,36 +734,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -776,26 +788,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1134,7 +1131,7 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D3" sqref="D3:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,654 +1146,654 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="C27" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="17"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="6" t="s">
+      <c r="B30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="18" t="s">
+      <c r="C30" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D30" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E30" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F30" s="9" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="12" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C31" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D31" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E31" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="F31" s="9" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C32" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D32" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E32" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F32" s="9" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C33" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D33" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E33" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F33" s="9" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C34" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D34" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E34" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F34" s="9" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
+      <c r="C36" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="E41" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="F41" s="23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="6" t="s">
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="6" t="s">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
@@ -1858,15 +1855,16 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:F22"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new stuff (and fixed #1)
</commit_message>
<xml_diff>
--- a/allData.xlsx
+++ b/allData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZakrzewskiJakub\source\repos\Zakrzewiaczek\Weather-Rider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F92743-AAC5-4201-9347-3E18BEA56EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA0FD45-289A-4755-AADB-8D8F3EC1460D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{501DA96D-EA6F-4FF1-BC3F-B1390DEB246D}"/>
+    <workbookView xWindow="15525" yWindow="0" windowWidth="13380" windowHeight="15585" xr2:uid="{501DA96D-EA6F-4FF1-BC3F-B1390DEB246D}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -1130,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CFDC78-4BA0-4FB0-8BF8-B8EE9309BE90}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D11"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>